<commit_message>
datya dysplay bworks with smoother, made test run tri work better
</commit_message>
<xml_diff>
--- a/ExamleExcel.xlsx
+++ b/ExamleExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programing\Actual programing\Personal\MetuProjektas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625A243D-1B3B-4F4A-914F-5509FB8CC75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4901BF-90F5-4866-8B79-D27095AE2DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Coordinates seperated by a space or a comma</t>
   </si>
@@ -33,28 +33,31 @@
     <t>Value</t>
   </si>
   <si>
-    <t>55.26581294956432, 20.993661174894704</t>
-  </si>
-  <si>
-    <t>55.34366870394346, 21.19268200150342</t>
-  </si>
-  <si>
-    <t>53.92205196159938, 23.78643337914364</t>
-  </si>
-  <si>
-    <t>55.03126443910766, 22.119114154674488</t>
-  </si>
-  <si>
-    <t>55.05759963641486, 22.030332560071013</t>
-  </si>
-  <si>
-    <t>56.145236829941275, 25.6700370489752</t>
-  </si>
-  <si>
-    <t>54.57749202622418, 25.761035555727705</t>
-  </si>
-  <si>
-    <t>53.97305954983385, 24.686908122180924</t>
+    <t>53.96692989779158, 25.416455740683055</t>
+  </si>
+  <si>
+    <t>56.44296749286285, 24.836864193327976</t>
+  </si>
+  <si>
+    <t>54.44296015829089, 22.740469234809616</t>
+  </si>
+  <si>
+    <t>53.96692989779158, 23.776334979018685</t>
+  </si>
+  <si>
+    <t>56.272170765510346, 21.235997558696436</t>
+  </si>
+  <si>
+    <t>55.30851893387957, 26.748283126094723</t>
+  </si>
+  <si>
+    <t>56.16245896219404, 25.909725142687375</t>
+  </si>
+  <si>
+    <t>54.75601343546629, 25.18349116638527</t>
+  </si>
+  <si>
+    <t>55.761087088687496, 22.701365275429193</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +433,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -438,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -446,7 +449,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>-4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -454,7 +457,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -462,7 +465,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -470,7 +473,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,7 +481,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -486,7 +489,15 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>